<commit_message>
aggiunto fumo e plot
</commit_message>
<xml_diff>
--- a/output/LUAD_statistics.xlsx
+++ b/output/LUAD_statistics.xlsx
@@ -54,15 +54,15 @@
     <t>capri_bic.SD.POSTERR</t>
   </si>
   <si>
+    <t>36</t>
+  </si>
+  <si>
     <t>11</t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
-    <t>36</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -261,25 +261,25 @@
     <t>69</t>
   </si>
   <si>
+    <t>Pattern OR_KRAS_TP53</t>
+  </si>
+  <si>
     <t>Pattern OR_STK11_TP53</t>
   </si>
   <si>
     <t>Pattern OR_CDK4_TP53</t>
   </si>
   <si>
-    <t>Pattern OR_KRAS_TP53</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
+    <t>Nonsense_Mutation RB1</t>
+  </si>
+  <si>
     <t>Del/Ins_Mutations KEAP1</t>
   </si>
   <si>
     <t>Missense_Mutation CDKN2A</t>
-  </si>
-  <si>
-    <t>Nonsense_Mutation RB1</t>
   </si>
   <si>
     <t>Amplification BRAF</t>
@@ -620,19 +620,19 @@
         <v>86</v>
       </c>
       <c r="D2" t="n">
-        <v>279.0</v>
+        <v>327.0</v>
       </c>
       <c r="E2" t="n">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.05</v>
+        <v>0.0382612502375296</v>
       </c>
       <c r="G2" t="n">
         <v>0.0318012848103768</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0</v>
+        <v>0.0317970902514371</v>
       </c>
       <c r="I2" t="n">
         <v>100.0</v>
@@ -640,14 +640,14 @@
       <c r="J2" t="n">
         <v>100.0</v>
       </c>
-      <c r="K2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="L2" t="e">
-        <v>#NUM!</v>
+      <c r="K2" t="n">
+        <v>0.021321961620469083</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0255863539445629</v>
+        <v>0.0213219616204691</v>
       </c>
       <c r="N2" t="n">
         <v>0.0</v>
@@ -664,34 +664,34 @@
         <v>87</v>
       </c>
       <c r="D3" t="n">
-        <v>242.0</v>
+        <v>279.0</v>
       </c>
       <c r="E3" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0382612502375296</v>
+        <v>0.05</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0382612502375296</v>
+        <v>0.0318012848103768</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0124042560537172</v>
+        <v>0.0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="J3" t="n">
         <v>100.0</v>
       </c>
-      <c r="K3" t="n">
-        <v>0.02771855010660981</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1.1564823173178713E-18</v>
+      <c r="K3" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="L3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0277185501066098</v>
+        <v>0.0255863539445629</v>
       </c>
       <c r="N3" t="n">
         <v>0.0</v>
@@ -708,19 +708,19 @@
         <v>88</v>
       </c>
       <c r="D4" t="n">
-        <v>327.0</v>
+        <v>242.0</v>
       </c>
       <c r="E4" t="n">
-        <v>10.0</v>
+        <v>13.0</v>
       </c>
       <c r="F4" t="n">
         <v>0.0382612502375296</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0318012848103768</v>
+        <v>0.0382612502375296</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0317970902514371</v>
+        <v>0.0124042560537172</v>
       </c>
       <c r="I4" t="n">
         <v>0.0</v>
@@ -729,16 +729,16 @@
         <v>100.0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.021321961620469083</v>
+        <v>0.02771855010660981</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0</v>
+        <v>1.1564823173178713E-18</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0213219616204691</v>
+        <v>0.0277185501066098</v>
       </c>
       <c r="N4" t="n">
-        <v>0.0</v>
+        <v>1.15648231731787E-18</v>
       </c>
     </row>
     <row r="5">
@@ -864,7 +864,7 @@
         <v>0.05543710021321962</v>
       </c>
       <c r="L7" t="n">
-        <v>3.271025955591198E-18</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M7" t="e">
         <v>#NUM!</v>
@@ -908,7 +908,7 @@
         <v>0.06183368869936034</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M8" t="e">
         <v>#NUM!</v>
@@ -1172,7 +1172,7 @@
         <v>0.1257995735607676</v>
       </c>
       <c r="L14" t="n">
-        <v>9.25185853854297E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M14" t="e">
         <v>#NUM!</v>
@@ -1392,7 +1392,7 @@
         <v>0.0255863539445629</v>
       </c>
       <c r="L19" t="n">
-        <v>0.0</v>
+        <v>1.1564823173178713E-18</v>
       </c>
       <c r="M19" t="e">
         <v>#NUM!</v>
@@ -1436,7 +1436,7 @@
         <v>0.05543710021321962</v>
       </c>
       <c r="L20" t="n">
-        <v>0.0</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M20" t="e">
         <v>#NUM!</v>
@@ -1700,7 +1700,7 @@
         <v>0.04477611940298507</v>
       </c>
       <c r="L26" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M26" t="e">
         <v>#NUM!</v>
@@ -1744,7 +1744,7 @@
         <v>0.05970149253731343</v>
       </c>
       <c r="L27" t="n">
-        <v>4.006172263299091E-18</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M27" t="e">
         <v>#NUM!</v>
@@ -1964,7 +1964,7 @@
         <v>0.04477611940298507</v>
       </c>
       <c r="L32" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M32" t="e">
         <v>#NUM!</v>
@@ -2228,7 +2228,7 @@
         <v>0.029850746268656716</v>
       </c>
       <c r="L38" t="n">
-        <v>1.635512977795599E-18</v>
+        <v>1.1564823173178713E-18</v>
       </c>
       <c r="M38" t="e">
         <v>#NUM!</v>
@@ -2404,7 +2404,7 @@
         <v>0.10021321961620469</v>
       </c>
       <c r="L42" t="n">
-        <v>0.0</v>
+        <v>4.625929269271485E-18</v>
       </c>
       <c r="M42" t="e">
         <v>#NUM!</v>
@@ -2641,7 +2641,7 @@
         <v>85</v>
       </c>
       <c r="C48" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D48" t="e">
         <v>#NUM!</v>
@@ -2665,10 +2665,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K48" t="n">
-        <v>0.49296375266524517</v>
+        <v>0.48848614072494667</v>
       </c>
       <c r="L48" t="n">
-        <v>0.019302624246502302</v>
+        <v>0.009768365059575655</v>
       </c>
       <c r="M48" t="e">
         <v>#NUM!</v>
@@ -2797,10 +2797,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K51" t="n">
-        <v>0.47761194029850745</v>
+        <v>0.47995735607675905</v>
       </c>
       <c r="L51" t="n">
-        <v>0.0</v>
+        <v>0.007416855919371459</v>
       </c>
       <c r="M51" t="e">
         <v>#NUM!</v>
@@ -2888,7 +2888,7 @@
         <v>0.2302771855010661</v>
       </c>
       <c r="L53" t="n">
-        <v>0.0</v>
+        <v>9.25185853854297E-18</v>
       </c>
       <c r="M53" t="e">
         <v>#NUM!</v>
@@ -2993,7 +2993,7 @@
         <v>85</v>
       </c>
       <c r="C56" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D56" t="e">
         <v>#NUM!</v>
@@ -3061,10 +3061,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K57" t="n">
-        <v>0.4859275053304904</v>
+        <v>0.5002132196162047</v>
       </c>
       <c r="L57" t="n">
-        <v>0.006068336661303939</v>
+        <v>0.025943180338795835</v>
       </c>
       <c r="M57" t="e">
         <v>#NUM!</v>
@@ -3240,7 +3240,7 @@
         <v>0.057569296375266525</v>
       </c>
       <c r="L61" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M61" t="e">
         <v>#NUM!</v>
@@ -3345,7 +3345,7 @@
         <v>85</v>
       </c>
       <c r="C64" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D64" t="e">
         <v>#NUM!</v>
@@ -3413,10 +3413,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K65" t="n">
-        <v>0.48187633262260127</v>
+        <v>0.48656716417910445</v>
       </c>
       <c r="L65" t="n">
-        <v>0.0</v>
+        <v>0.01109288586503294</v>
       </c>
       <c r="M65" t="e">
         <v>#NUM!</v>
@@ -3460,7 +3460,7 @@
         <v>0.0511727078891258</v>
       </c>
       <c r="L66" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M66" t="e">
         <v>#NUM!</v>
@@ -3548,7 +3548,7 @@
         <v>0.053304904051172705</v>
       </c>
       <c r="L68" t="n">
-        <v>3.271025955591198E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M68" t="e">
         <v>#NUM!</v>
@@ -3702,7 +3702,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>82</v>
@@ -3711,19 +3711,19 @@
         <v>86</v>
       </c>
       <c r="D2" t="n">
-        <v>279.0</v>
+        <v>327.0</v>
       </c>
       <c r="E2" t="n">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.05</v>
+        <v>0.0382612502375296</v>
       </c>
       <c r="G2" t="n">
         <v>0.0318012848103768</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0</v>
+        <v>0.0317970902514371</v>
       </c>
       <c r="I2" t="n">
         <v>100.0</v>
@@ -3731,14 +3731,14 @@
       <c r="J2" t="n">
         <v>100.0</v>
       </c>
-      <c r="K2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="L2" t="e">
-        <v>#NUM!</v>
+      <c r="K2" t="n">
+        <v>0.021321961620469083</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.0</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0255863539445629</v>
+        <v>0.0213219616204691</v>
       </c>
       <c r="N2" t="n">
         <v>0.0</v>
@@ -3746,72 +3746,72 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D3" t="n">
-        <v>242.0</v>
+        <v>279.0</v>
       </c>
       <c r="E3" t="n">
-        <v>26.0</v>
+        <v>12.0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0382612502375296</v>
+        <v>0.05</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0382612502375296</v>
+        <v>0.0318012848103768</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0485467857697238</v>
+        <v>0.0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.05543710021321962</v>
-      </c>
-      <c r="L3" t="n">
-        <v>3.271025955591198E-18</v>
+        <v>100.0</v>
+      </c>
+      <c r="K3" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="L3" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="M3" t="n">
-        <v>0.0554371002132196</v>
+        <v>0.0255863539445629</v>
       </c>
       <c r="N3" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D4" t="n">
-        <v>11.0</v>
+        <v>242.0</v>
       </c>
       <c r="E4" t="n">
         <v>26.0</v>
       </c>
       <c r="F4" t="n">
-        <v>1.0</v>
+        <v>0.0382612502375296</v>
       </c>
       <c r="G4" t="n">
         <v>0.0382612502375296</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0671688978580581</v>
+        <v>0.0485467857697238</v>
       </c>
       <c r="I4" t="n">
         <v>0.0</v>
@@ -3823,7 +3823,7 @@
         <v>0.05543710021321962</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M4" t="n">
         <v>0.0554371002132196</v>
@@ -3834,28 +3834,28 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>95</v>
       </c>
       <c r="D5" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="E5" t="n">
         <v>26.0</v>
       </c>
-      <c r="E5" t="n">
-        <v>10.0</v>
-      </c>
       <c r="F5" t="n">
-        <v>0.0360990988508288</v>
+        <v>1.0</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0360990988508288</v>
+        <v>0.0382612502375296</v>
       </c>
       <c r="H5" t="n">
-        <v>0.15187893000577601</v>
+        <v>0.0671688978580581</v>
       </c>
       <c r="I5" t="n">
         <v>0.0</v>
@@ -3863,14 +3863,14 @@
       <c r="J5" t="n">
         <v>0.0</v>
       </c>
-      <c r="K5" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="L5" t="e">
-        <v>#NUM!</v>
+      <c r="K5" t="n">
+        <v>0.05543710021321962</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0213219616204691</v>
+        <v>0.0554371002132196</v>
       </c>
       <c r="N5" t="n">
         <v>0.0</v>
@@ -3878,28 +3878,28 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C6" t="s">
         <v>167</v>
       </c>
       <c r="D6" t="n">
-        <v>16.0</v>
+        <v>26.0</v>
       </c>
       <c r="E6" t="n">
         <v>10.0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0382612502375296</v>
+        <v>0.0360990988508288</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0382612502375296</v>
+        <v>0.0360990988508288</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0894072382163834</v>
+        <v>0.15187893000577601</v>
       </c>
       <c r="I6" t="n">
         <v>0.0</v>
@@ -3922,19 +3922,19 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>167</v>
       </c>
       <c r="D7" t="n">
-        <v>242.0</v>
+        <v>16.0</v>
       </c>
       <c r="E7" t="n">
-        <v>13.0</v>
+        <v>10.0</v>
       </c>
       <c r="F7" t="n">
         <v>0.0382612502375296</v>
@@ -3943,22 +3943,22 @@
         <v>0.0382612502375296</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0124042560537172</v>
+        <v>0.0894072382163834</v>
       </c>
       <c r="I7" t="n">
         <v>0.0</v>
       </c>
       <c r="J7" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.02771855010660981</v>
-      </c>
-      <c r="L7" t="n">
-        <v>1.1564823173178713E-18</v>
+        <v>0.0</v>
+      </c>
+      <c r="K7" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="L7" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="M7" t="n">
-        <v>0.0277185501066098</v>
+        <v>0.0213219616204691</v>
       </c>
       <c r="N7" t="n">
         <v>0.0</v>
@@ -3966,87 +3966,87 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="C8" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="D8" t="n">
-        <v>11.0</v>
+        <v>242.0</v>
       </c>
       <c r="E8" t="n">
-        <v>16.0</v>
+        <v>13.0</v>
       </c>
       <c r="F8" t="n">
-        <v>1.0</v>
+        <v>0.0382612502375296</v>
       </c>
       <c r="G8" t="n">
         <v>0.0382612502375296</v>
       </c>
       <c r="H8" t="n">
-        <v>3.95644774502605E-4</v>
+        <v>0.0124042560537172</v>
       </c>
       <c r="I8" t="n">
         <v>0.0</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0</v>
+        <v>100.0</v>
       </c>
       <c r="K8" t="n">
-        <v>0.03411513859275053</v>
+        <v>0.02771855010660981</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0</v>
+        <v>1.1564823173178713E-18</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0341151385927505</v>
+        <v>0.0277185501066098</v>
       </c>
       <c r="N8" t="n">
-        <v>0.0</v>
+        <v>1.15648231731787E-18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="D9" t="n">
-        <v>327.0</v>
+        <v>11.0</v>
       </c>
       <c r="E9" t="n">
-        <v>10.0</v>
+        <v>16.0</v>
       </c>
       <c r="F9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="G9" t="n">
         <v>0.0382612502375296</v>
       </c>
-      <c r="G9" t="n">
-        <v>0.0318012848103768</v>
-      </c>
       <c r="H9" t="n">
-        <v>0.0317970902514371</v>
+        <v>3.95644774502605E-4</v>
       </c>
       <c r="I9" t="n">
         <v>0.0</v>
       </c>
       <c r="J9" t="n">
-        <v>100.0</v>
+        <v>0.0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.021321961620469083</v>
+        <v>0.03411513859275053</v>
       </c>
       <c r="L9" t="n">
         <v>0.0</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0213219616204691</v>
+        <v>0.0341151385927505</v>
       </c>
       <c r="N9" t="n">
         <v>0.0</v>
@@ -4134,10 +4134,10 @@
         <v>0.0</v>
       </c>
       <c r="M11" t="n">
-        <v>0.198720682302772</v>
+        <v>0.201492537313433</v>
       </c>
       <c r="N11" t="n">
-        <v>0.00386680042892265</v>
+        <v>0.00365871717874449</v>
       </c>
     </row>
     <row r="12">
@@ -4175,13 +4175,13 @@
         <v>0.057569296375266525</v>
       </c>
       <c r="L12" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M12" t="n">
         <v>0.0575692963752665</v>
       </c>
       <c r="N12" t="n">
-        <v>3.2710259555912E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="13">
@@ -4219,7 +4219,7 @@
         <v>0.0511727078891258</v>
       </c>
       <c r="L13" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M13" t="n">
         <v>0.0511727078891258</v>
@@ -4351,7 +4351,7 @@
         <v>0.06183368869936034</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M16" t="e">
         <v>#NUM!</v>
@@ -4571,7 +4571,7 @@
         <v>0.1257995735607676</v>
       </c>
       <c r="L21" t="n">
-        <v>9.25185853854297E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M21" t="e">
         <v>#NUM!</v>
@@ -4791,7 +4791,7 @@
         <v>0.0255863539445629</v>
       </c>
       <c r="L26" t="n">
-        <v>0.0</v>
+        <v>1.1564823173178713E-18</v>
       </c>
       <c r="M26" t="e">
         <v>#NUM!</v>
@@ -4802,7 +4802,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
         <v>85</v>
@@ -4835,7 +4835,7 @@
         <v>0.05543710021321962</v>
       </c>
       <c r="L27" t="n">
-        <v>0.0</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M27" t="e">
         <v>#NUM!</v>
@@ -5099,7 +5099,7 @@
         <v>0.04477611940298507</v>
       </c>
       <c r="L33" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M33" t="e">
         <v>#NUM!</v>
@@ -5143,7 +5143,7 @@
         <v>0.05970149253731343</v>
       </c>
       <c r="L34" t="n">
-        <v>4.006172263299091E-18</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M34" t="e">
         <v>#NUM!</v>
@@ -5319,7 +5319,7 @@
         <v>0.04477611940298507</v>
       </c>
       <c r="L38" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M38" t="e">
         <v>#NUM!</v>
@@ -5462,7 +5462,7 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B42" t="s">
         <v>85</v>
@@ -5583,7 +5583,7 @@
         <v>0.029850746268656716</v>
       </c>
       <c r="L44" t="n">
-        <v>1.635512977795599E-18</v>
+        <v>1.1564823173178713E-18</v>
       </c>
       <c r="M44" t="e">
         <v>#NUM!</v>
@@ -5715,7 +5715,7 @@
         <v>0.10021321961620469</v>
       </c>
       <c r="L47" t="n">
-        <v>0.0</v>
+        <v>4.625929269271485E-18</v>
       </c>
       <c r="M47" t="e">
         <v>#NUM!</v>
@@ -5952,7 +5952,7 @@
         <v>85</v>
       </c>
       <c r="C53" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D53" t="e">
         <v>#NUM!</v>
@@ -5976,10 +5976,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K53" t="n">
-        <v>0.49296375266524517</v>
+        <v>0.48848614072494667</v>
       </c>
       <c r="L53" t="n">
-        <v>0.019302624246502302</v>
+        <v>0.009768365059575655</v>
       </c>
       <c r="M53" t="e">
         <v>#NUM!</v>
@@ -6064,10 +6064,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K55" t="n">
-        <v>0.47761194029850745</v>
+        <v>0.47995735607675905</v>
       </c>
       <c r="L55" t="n">
-        <v>0.0</v>
+        <v>0.007416855919371459</v>
       </c>
       <c r="M55" t="e">
         <v>#NUM!</v>
@@ -6155,7 +6155,7 @@
         <v>0.2302771855010661</v>
       </c>
       <c r="L57" t="n">
-        <v>0.0</v>
+        <v>9.25185853854297E-18</v>
       </c>
       <c r="M57" t="e">
         <v>#NUM!</v>
@@ -6260,7 +6260,7 @@
         <v>85</v>
       </c>
       <c r="C60" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D60" t="e">
         <v>#NUM!</v>
@@ -6328,10 +6328,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K61" t="n">
-        <v>0.4859275053304904</v>
+        <v>0.5002132196162047</v>
       </c>
       <c r="L61" t="n">
-        <v>0.006068336661303939</v>
+        <v>0.025943180338795835</v>
       </c>
       <c r="M61" t="e">
         <v>#NUM!</v>
@@ -6568,7 +6568,7 @@
         <v>85</v>
       </c>
       <c r="C67" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D67" t="e">
         <v>#NUM!</v>
@@ -6636,10 +6636,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K68" t="n">
-        <v>0.48187633262260127</v>
+        <v>0.48656716417910445</v>
       </c>
       <c r="L68" t="n">
-        <v>0.0</v>
+        <v>0.01109288586503294</v>
       </c>
       <c r="M68" t="e">
         <v>#NUM!</v>
@@ -6727,7 +6727,7 @@
         <v>0.053304904051172705</v>
       </c>
       <c r="L70" t="n">
-        <v>3.271025955591198E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M70" t="e">
         <v>#NUM!</v>

</xml_diff>

<commit_message>
code refactoring - models and statistics removed
</commit_message>
<xml_diff>
--- a/output/LUAD_statistics.xlsx
+++ b/output/LUAD_statistics.xlsx
@@ -60,54 +60,54 @@
     <t>28</t>
   </si>
   <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
     <t>37</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>35</t>
+    <t>4</t>
   </si>
   <si>
     <t>34</t>
   </si>
   <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
     <t>31</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>14</t>
+    <t>30</t>
   </si>
   <si>
     <t>11</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
@@ -216,36 +216,36 @@
     <t>Mutation TP53</t>
   </si>
   <si>
+    <t>Pattern OR_CDK4_TP53</t>
+  </si>
+  <si>
+    <t>Amplification CDK4</t>
+  </si>
+  <si>
+    <t>Mutation KRAS</t>
+  </si>
+  <si>
+    <t>Pattern OR_CDKN2A</t>
+  </si>
+  <si>
+    <t>Mutation ATM</t>
+  </si>
+  <si>
+    <t>Mutation SMARCA4</t>
+  </si>
+  <si>
+    <t>Pattern OR_KRAS</t>
+  </si>
+  <si>
     <t>Mutation ARID2</t>
   </si>
   <si>
-    <t>Pattern OR_CDK4_TP53</t>
-  </si>
-  <si>
-    <t>Amplification CDK4</t>
-  </si>
-  <si>
-    <t>Mutation SMARCA4</t>
-  </si>
-  <si>
-    <t>Pattern OR_CDKN2A</t>
-  </si>
-  <si>
-    <t>Mutation KRAS</t>
-  </si>
-  <si>
-    <t>Pattern OR_KRAS</t>
+    <t>Amplification KRAS</t>
   </si>
   <si>
     <t>Mutation KEAP1</t>
   </si>
   <si>
-    <t>Mutation ATM</t>
-  </si>
-  <si>
-    <t>Amplification KRAS</t>
-  </si>
-  <si>
     <t>Mutation ROS1</t>
   </si>
   <si>
@@ -261,33 +261,33 @@
     <t>Mutation RB1</t>
   </si>
   <si>
+    <t>Amplification MDM2</t>
+  </si>
+  <si>
+    <t>Amplification CCND1</t>
+  </si>
+  <si>
+    <t>Mutation NFE2L2</t>
+  </si>
+  <si>
+    <t>Mutation STK11</t>
+  </si>
+  <si>
     <t>Pattern AND_PIK3CA_RB1</t>
   </si>
   <si>
-    <t>Amplification MDM2</t>
-  </si>
-  <si>
-    <t>Mutation NFE2L2</t>
-  </si>
-  <si>
-    <t>Amplification CCND1</t>
-  </si>
-  <si>
-    <t>Mutation STK11</t>
+    <t>Mutation CDKN2A</t>
   </si>
   <si>
     <t>Mutation ARID1B</t>
   </si>
   <si>
+    <t>Mutation RET</t>
+  </si>
+  <si>
     <t>Deletion CDKN2A</t>
   </si>
   <si>
-    <t>Mutation CDKN2A</t>
-  </si>
-  <si>
-    <t>Mutation RET</t>
-  </si>
-  <si>
     <t>Amplification MET</t>
   </si>
   <si>
@@ -399,10 +399,10 @@
     <t>capri_aic.SD.POSTERR</t>
   </si>
   <si>
+    <t>58</t>
+  </si>
+  <si>
     <t>60</t>
-  </si>
-  <si>
-    <t>58</t>
   </si>
   <si>
     <t>57</t>
@@ -596,7 +596,7 @@
         <v>0.05919661733615222</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M2" t="n">
         <v>0.0591966173361522</v>
@@ -631,7 +631,7 @@
         <v>2.85337647084671E-6</v>
       </c>
       <c r="I3" t="n">
-        <v>90.0</v>
+        <v>95.0</v>
       </c>
       <c r="J3" t="n">
         <v>100.0</v>
@@ -640,13 +640,13 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L3" t="n">
-        <v>6.542051911182396E-18</v>
+        <v>8.012344526598183E-18</v>
       </c>
       <c r="M3" t="n">
         <v>0.06553911205074</v>
       </c>
       <c r="N3" t="n">
-        <v>6.5420519111824E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
@@ -657,40 +657,40 @@
         <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D4" t="n">
-        <v>32.0</v>
+        <v>265.0</v>
       </c>
       <c r="E4" t="n">
-        <v>2.0</v>
+        <v>28.0</v>
       </c>
       <c r="F4" t="n">
-        <v>4.4059017720226E-40</v>
+        <v>6.6780646105007E-40</v>
       </c>
       <c r="G4" t="n">
-        <v>2.80388279688621E-39</v>
+        <v>7.22240061663926E-40</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0</v>
+        <v>2.35123065785807E-6</v>
       </c>
       <c r="I4" t="n">
-        <v>72.0</v>
+        <v>74.0</v>
       </c>
       <c r="J4" t="n">
         <v>100.0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.004228329809725159</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M4" t="n">
-        <v>0.00422832980972516</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N4" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="5">
@@ -701,37 +701,37 @@
         <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D5" t="n">
-        <v>265.0</v>
+        <v>29.0</v>
       </c>
       <c r="E5" t="n">
-        <v>28.0</v>
+        <v>26.0</v>
       </c>
       <c r="F5" t="n">
-        <v>6.6780646105007E-40</v>
+        <v>4.2567941954014E-4</v>
       </c>
       <c r="G5" t="n">
-        <v>7.22240061663926E-40</v>
+        <v>7.27855148517323E-40</v>
       </c>
       <c r="H5" t="n">
-        <v>2.35123065785807E-6</v>
+        <v>1.34895703589137E-9</v>
       </c>
       <c r="I5" t="n">
-        <v>70.0</v>
+        <v>72.0</v>
       </c>
       <c r="J5" t="n">
         <v>100.0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L5" t="n">
         <v>0.0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N5" t="n">
         <v>2.31296463463574E-18</v>
@@ -745,37 +745,37 @@
         <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D6" t="n">
-        <v>29.0</v>
+        <v>141.0</v>
       </c>
       <c r="E6" t="n">
-        <v>26.0</v>
+        <v>34.0</v>
       </c>
       <c r="F6" t="n">
-        <v>4.2567941954014E-4</v>
+        <v>6.91424234824968E-40</v>
       </c>
       <c r="G6" t="n">
-        <v>7.27855148517323E-40</v>
+        <v>5.22572749966404E-38</v>
       </c>
       <c r="H6" t="n">
-        <v>1.34895703589137E-9</v>
+        <v>0.00511448636585391</v>
       </c>
       <c r="I6" t="n">
-        <v>65.0</v>
+        <v>66.0</v>
       </c>
       <c r="J6" t="n">
         <v>100.0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L6" t="n">
         <v>0.0</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0549682875264271</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N6" t="n">
         <v>0.0</v>
@@ -789,37 +789,37 @@
         <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D7" t="n">
-        <v>48.0</v>
+        <v>103.0</v>
       </c>
       <c r="E7" t="n">
-        <v>15.0</v>
+        <v>19.0</v>
       </c>
       <c r="F7" t="n">
-        <v>6.35703372325376E-40</v>
+        <v>6.51999369723878E-40</v>
       </c>
       <c r="G7" t="n">
-        <v>5.55194292468331E-38</v>
+        <v>1.25468290861042E-39</v>
       </c>
       <c r="H7" t="n">
-        <v>0.00198021340048057</v>
+        <v>4.62499234591398E-4</v>
       </c>
       <c r="I7" t="n">
-        <v>64.0</v>
+        <v>65.0</v>
       </c>
       <c r="J7" t="n">
         <v>100.0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="L7" t="n">
         <v>0.0</v>
       </c>
       <c r="M7" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N7" t="n">
         <v>0.0</v>
@@ -833,25 +833,25 @@
         <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D8" t="n">
-        <v>103.0</v>
+        <v>46.0</v>
       </c>
       <c r="E8" t="n">
         <v>19.0</v>
       </c>
       <c r="F8" t="n">
-        <v>6.51999369723878E-40</v>
+        <v>6.37169273862073E-40</v>
       </c>
       <c r="G8" t="n">
-        <v>1.25468290861042E-39</v>
+        <v>4.50672171343806E-36</v>
       </c>
       <c r="H8" t="n">
-        <v>4.62499234591398E-4</v>
+        <v>0.00625718664081437</v>
       </c>
       <c r="I8" t="n">
-        <v>62.0</v>
+        <v>63.0</v>
       </c>
       <c r="J8" t="n">
         <v>100.0</v>
@@ -877,37 +877,37 @@
         <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="D9" t="n">
-        <v>141.0</v>
+        <v>48.0</v>
       </c>
       <c r="E9" t="n">
-        <v>34.0</v>
+        <v>15.0</v>
       </c>
       <c r="F9" t="n">
-        <v>6.91424234824968E-40</v>
+        <v>6.35703372325376E-40</v>
       </c>
       <c r="G9" t="n">
-        <v>5.22572749966404E-38</v>
+        <v>5.55194292468331E-38</v>
       </c>
       <c r="H9" t="n">
-        <v>0.00511448636585391</v>
+        <v>0.00198021340048057</v>
       </c>
       <c r="I9" t="n">
-        <v>55.0</v>
+        <v>62.0</v>
       </c>
       <c r="J9" t="n">
         <v>100.0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L9" t="n">
         <v>0.0</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N9" t="n">
         <v>0.0</v>
@@ -921,37 +921,37 @@
         <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="D10" t="n">
         <v>158.0</v>
       </c>
       <c r="E10" t="n">
-        <v>84.0</v>
+        <v>46.0</v>
       </c>
       <c r="F10" t="n">
-        <v>7.04377675145043E-40</v>
+        <v>6.81212204280953E-40</v>
       </c>
       <c r="G10" t="n">
-        <v>7.48419636793941E-40</v>
+        <v>1.08858185548109E-39</v>
       </c>
       <c r="H10" t="n">
-        <v>8.72881864945047E-5</v>
+        <v>5.24181844605938E-4</v>
       </c>
       <c r="I10" t="n">
-        <v>53.0</v>
+        <v>60.0</v>
       </c>
       <c r="J10" t="n">
         <v>100.0</v>
       </c>
       <c r="K10" t="n">
-        <v>0.179492600422833</v>
+        <v>0.09725158562367865</v>
       </c>
       <c r="L10" t="n">
-        <v>0.004280857659897791</v>
+        <v>0.0</v>
       </c>
       <c r="M10" t="n">
-        <v>0.177589852008457</v>
+        <v>0.0972515856236787</v>
       </c>
       <c r="N10" t="n">
         <v>0.0</v>
@@ -962,37 +962,37 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" t="n">
-        <v>93.0</v>
+        <v>158.0</v>
       </c>
       <c r="E11" t="n">
         <v>84.0</v>
       </c>
       <c r="F11" t="n">
-        <v>4.10865511869097E-15</v>
+        <v>7.04377675145043E-40</v>
       </c>
       <c r="G11" t="n">
-        <v>7.29044301902058E-40</v>
+        <v>7.48419636793941E-40</v>
       </c>
       <c r="H11" t="n">
-        <v>2.66335709542836E-4</v>
+        <v>8.72881864945047E-5</v>
       </c>
       <c r="I11" t="n">
-        <v>49.0</v>
+        <v>50.0</v>
       </c>
       <c r="J11" t="n">
         <v>100.0</v>
       </c>
       <c r="K11" t="n">
-        <v>0.179492600422833</v>
+        <v>0.17716701902748416</v>
       </c>
       <c r="L11" t="n">
-        <v>0.004280857659897791</v>
+        <v>0.0013371152897117948</v>
       </c>
       <c r="M11" t="n">
         <v>0.177589852008457</v>
@@ -1006,43 +1006,43 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="D12" t="n">
-        <v>250.0</v>
+        <v>32.0</v>
       </c>
       <c r="E12" t="n">
-        <v>26.0</v>
+        <v>2.0</v>
       </c>
       <c r="F12" t="n">
-        <v>6.81526409297973E-40</v>
+        <v>4.4059017720226E-40</v>
       </c>
       <c r="G12" t="n">
-        <v>1.07501177508528E-39</v>
+        <v>2.80388279688621E-39</v>
       </c>
       <c r="H12" t="n">
-        <v>0.00244603283957377</v>
+        <v>0.0</v>
       </c>
       <c r="I12" t="n">
-        <v>47.0</v>
+        <v>49.0</v>
       </c>
       <c r="J12" t="n">
         <v>100.0</v>
       </c>
       <c r="K12" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.004228329809725159</v>
       </c>
       <c r="L12" t="n">
         <v>0.0</v>
       </c>
       <c r="M12" t="n">
-        <v>0.0549682875264271</v>
+        <v>0.00422832980972516</v>
       </c>
       <c r="N12" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="13">
@@ -1053,37 +1053,37 @@
         <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="D13" t="n">
-        <v>46.0</v>
+        <v>34.0</v>
       </c>
       <c r="E13" t="n">
-        <v>19.0</v>
+        <v>29.0</v>
       </c>
       <c r="F13" t="n">
-        <v>6.37169273862073E-40</v>
+        <v>1.93777120033396E-6</v>
       </c>
       <c r="G13" t="n">
-        <v>4.50672171343806E-36</v>
+        <v>7.27702830087346E-40</v>
       </c>
       <c r="H13" t="n">
-        <v>0.00625718664081437</v>
+        <v>4.85557252274751E-5</v>
       </c>
       <c r="I13" t="n">
-        <v>46.0</v>
+        <v>47.0</v>
       </c>
       <c r="J13" t="n">
         <v>100.0</v>
       </c>
       <c r="K13" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0613107822410148</v>
       </c>
       <c r="L13" t="n">
         <v>0.0</v>
       </c>
       <c r="M13" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0613107822410148</v>
       </c>
       <c r="N13" t="n">
         <v>0.0</v>
@@ -1094,25 +1094,25 @@
         <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="D14" t="n">
-        <v>158.0</v>
+        <v>93.0</v>
       </c>
       <c r="E14" t="n">
-        <v>46.0</v>
+        <v>84.0</v>
       </c>
       <c r="F14" t="n">
-        <v>6.81212204280953E-40</v>
+        <v>4.10865511869097E-15</v>
       </c>
       <c r="G14" t="n">
-        <v>1.08858185548109E-39</v>
+        <v>7.29044301902058E-40</v>
       </c>
       <c r="H14" t="n">
-        <v>5.24181844605938E-4</v>
+        <v>2.66335709542836E-4</v>
       </c>
       <c r="I14" t="n">
         <v>45.0</v>
@@ -1121,13 +1121,13 @@
         <v>100.0</v>
       </c>
       <c r="K14" t="n">
-        <v>0.09725158562367865</v>
+        <v>0.17716701902748416</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0</v>
+        <v>0.0013371152897117948</v>
       </c>
       <c r="M14" t="n">
-        <v>0.0972515856236787</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N14" t="n">
         <v>0.0</v>
@@ -1138,40 +1138,40 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="D15" t="n">
-        <v>34.0</v>
+        <v>250.0</v>
       </c>
       <c r="E15" t="n">
-        <v>29.0</v>
+        <v>25.0</v>
       </c>
       <c r="F15" t="n">
-        <v>1.93777120033396E-6</v>
+        <v>6.73035927110432E-40</v>
       </c>
       <c r="G15" t="n">
-        <v>7.27702830087346E-40</v>
+        <v>1.04706416839736E-39</v>
       </c>
       <c r="H15" t="n">
-        <v>4.85557252274751E-5</v>
+        <v>9.10299739159604E-4</v>
       </c>
       <c r="I15" t="n">
-        <v>44.0</v>
+        <v>22.0</v>
       </c>
       <c r="J15" t="n">
         <v>100.0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.0613107822410148</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L15" t="n">
         <v>0.0</v>
       </c>
       <c r="M15" t="n">
-        <v>0.0613107822410148</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N15" t="n">
         <v>0.0</v>
@@ -1185,7 +1185,7 @@
         <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D16" t="n">
         <v>26.0</v>
@@ -1203,7 +1203,7 @@
         <v>1.57998188512074E-5</v>
       </c>
       <c r="I16" t="n">
-        <v>41.0</v>
+        <v>21.0</v>
       </c>
       <c r="J16" t="n">
         <v>100.0</v>
@@ -1212,7 +1212,7 @@
         <v>0.052854122621564484</v>
       </c>
       <c r="L16" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M16" t="n">
         <v>0.0528541226215645</v>
@@ -1226,40 +1226,40 @@
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D17" t="n">
-        <v>120.0</v>
+        <v>250.0</v>
       </c>
       <c r="E17" t="n">
-        <v>82.0</v>
+        <v>26.0</v>
       </c>
       <c r="F17" t="n">
-        <v>8.41039238887027E-40</v>
+        <v>6.81526409297973E-40</v>
       </c>
       <c r="G17" t="n">
-        <v>7.87697455852087E-40</v>
+        <v>1.07501177508528E-39</v>
       </c>
       <c r="H17" t="n">
-        <v>7.20794801965287E-4</v>
+        <v>0.00244603283957377</v>
       </c>
       <c r="I17" t="n">
-        <v>30.0</v>
+        <v>20.0</v>
       </c>
       <c r="J17" t="n">
         <v>100.0</v>
       </c>
       <c r="K17" t="n">
-        <v>0.1733615221987315</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L17" t="n">
         <v>0.0</v>
       </c>
       <c r="M17" t="n">
-        <v>0.173361522198731</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N17" t="n">
         <v>0.0</v>
@@ -1270,40 +1270,40 @@
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
         <v>89</v>
       </c>
       <c r="D18" t="n">
-        <v>250.0</v>
+        <v>265.0</v>
       </c>
       <c r="E18" t="n">
-        <v>25.0</v>
+        <v>23.0</v>
       </c>
       <c r="F18" t="n">
-        <v>6.73035927110432E-40</v>
+        <v>6.71457268463716E-40</v>
       </c>
       <c r="G18" t="n">
-        <v>1.04706416839736E-39</v>
+        <v>7.27946554528017E-40</v>
       </c>
       <c r="H18" t="n">
-        <v>9.10299739159604E-4</v>
+        <v>2.31452640435795E-4</v>
       </c>
       <c r="I18" t="n">
-        <v>24.0</v>
+        <v>18.0</v>
       </c>
       <c r="J18" t="n">
         <v>100.0</v>
       </c>
       <c r="K18" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.048625792811839326</v>
       </c>
       <c r="L18" t="n">
         <v>0.0</v>
       </c>
       <c r="M18" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.0486257928118393</v>
       </c>
       <c r="N18" t="n">
         <v>0.0</v>
@@ -1314,40 +1314,40 @@
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
         <v>90</v>
       </c>
       <c r="D19" t="n">
-        <v>265.0</v>
+        <v>120.0</v>
       </c>
       <c r="E19" t="n">
-        <v>23.0</v>
+        <v>82.0</v>
       </c>
       <c r="F19" t="n">
-        <v>6.71457268463716E-40</v>
+        <v>8.41039238887027E-40</v>
       </c>
       <c r="G19" t="n">
-        <v>7.27946554528017E-40</v>
+        <v>7.87697455852087E-40</v>
       </c>
       <c r="H19" t="n">
-        <v>2.31452640435795E-4</v>
+        <v>7.20794801965287E-4</v>
       </c>
       <c r="I19" t="n">
-        <v>22.0</v>
+        <v>14.0</v>
       </c>
       <c r="J19" t="n">
         <v>100.0</v>
       </c>
       <c r="K19" t="n">
-        <v>0.048625792811839326</v>
+        <v>0.1733615221987315</v>
       </c>
       <c r="L19" t="n">
         <v>0.0</v>
       </c>
       <c r="M19" t="n">
-        <v>0.0486257928118393</v>
+        <v>0.173361522198731</v>
       </c>
       <c r="N19" t="n">
         <v>0.0</v>
@@ -1358,7 +1358,7 @@
         <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
         <v>91</v>
@@ -1379,7 +1379,7 @@
         <v>0.00115041602190713</v>
       </c>
       <c r="I20" t="n">
-        <v>18.0</v>
+        <v>9.0</v>
       </c>
       <c r="J20" t="n">
         <v>100.0</v>
@@ -1564,7 +1564,7 @@
         <v>0.05919661733615222</v>
       </c>
       <c r="L24" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M24" t="e">
         <v>#NUM!</v>
@@ -1581,7 +1581,7 @@
         <v>79</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D25" t="e">
         <v>#NUM!</v>
@@ -1608,7 +1608,7 @@
         <v>0.06765327695560254</v>
       </c>
       <c r="L25" t="n">
-        <v>6.542051911182396E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M25" t="e">
         <v>#NUM!</v>
@@ -1757,7 +1757,7 @@
         <v>79</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D29" t="e">
         <v>#NUM!</v>
@@ -1801,7 +1801,7 @@
         <v>79</v>
       </c>
       <c r="C30" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D30" t="e">
         <v>#NUM!</v>
@@ -1916,7 +1916,7 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L32" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>8.012344526598183E-18</v>
       </c>
       <c r="M32" t="e">
         <v>#NUM!</v>
@@ -2004,7 +2004,7 @@
         <v>0.05708245243128964</v>
       </c>
       <c r="L34" t="n">
-        <v>0.0</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M34" t="e">
         <v>#NUM!</v>
@@ -2109,7 +2109,7 @@
         <v>79</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D37" t="e">
         <v>#NUM!</v>
@@ -2285,7 +2285,7 @@
         <v>79</v>
       </c>
       <c r="C41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D41" t="e">
         <v>#NUM!</v>
@@ -2329,7 +2329,7 @@
         <v>79</v>
       </c>
       <c r="C42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D42" t="e">
         <v>#NUM!</v>
@@ -2441,10 +2441,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K44" t="n">
-        <v>0.48414376321353064</v>
+        <v>0.49217758985200843</v>
       </c>
       <c r="L44" t="n">
-        <v>0.0</v>
+        <v>0.01693679366968268</v>
       </c>
       <c r="M44" t="e">
         <v>#NUM!</v>
@@ -2906,7 +2906,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>65</v>
@@ -2939,13 +2939,13 @@
         <v>0.05919661733615222</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M2" t="n">
-        <v>0.125581395348837</v>
+        <v>0.12093023255814</v>
       </c>
       <c r="N2" t="n">
-        <v>0.00662588260664871</v>
+        <v>0.00596312778049505</v>
       </c>
     </row>
     <row r="3">
@@ -2974,7 +2974,7 @@
         <v>2.85337647084671E-6</v>
       </c>
       <c r="I3" t="n">
-        <v>90.0</v>
+        <v>95.0</v>
       </c>
       <c r="J3" t="n">
         <v>100.0</v>
@@ -2983,186 +2983,186 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L3" t="n">
-        <v>6.542051911182396E-18</v>
+        <v>8.012344526598183E-18</v>
       </c>
       <c r="M3" t="n">
         <v>0.06553911205074</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0</v>
+        <v>4.62592926927149E-18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D4" t="n">
-        <v>32.0</v>
+        <v>265.0</v>
       </c>
       <c r="E4" t="n">
-        <v>2.0</v>
+        <v>28.0</v>
       </c>
       <c r="F4" t="n">
-        <v>4.4059017720226E-40</v>
+        <v>6.6780646105007E-40</v>
       </c>
       <c r="G4" t="n">
-        <v>2.80388279688621E-39</v>
+        <v>7.22240061663926E-40</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0</v>
+        <v>2.35123065785807E-6</v>
       </c>
       <c r="I4" t="n">
-        <v>72.0</v>
+        <v>74.0</v>
       </c>
       <c r="J4" t="n">
         <v>100.0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.004228329809725159</v>
+        <v>0.05919661733615222</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M4" t="n">
-        <v>0.00422832980972516</v>
+        <v>0.0591966173361522</v>
       </c>
       <c r="N4" t="n">
-        <v>0.0</v>
+        <v>3.2710259555912E-18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D5" t="n">
-        <v>265.0</v>
+        <v>29.0</v>
       </c>
       <c r="E5" t="n">
-        <v>28.0</v>
+        <v>26.0</v>
       </c>
       <c r="F5" t="n">
-        <v>6.6780646105007E-40</v>
+        <v>4.2567941954014E-4</v>
       </c>
       <c r="G5" t="n">
-        <v>7.22240061663926E-40</v>
+        <v>7.27855148517323E-40</v>
       </c>
       <c r="H5" t="n">
-        <v>2.35123065785807E-6</v>
+        <v>1.34895703589137E-9</v>
       </c>
       <c r="I5" t="n">
-        <v>70.0</v>
+        <v>72.0</v>
       </c>
       <c r="J5" t="n">
         <v>100.0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.05919661733615222</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L5" t="n">
         <v>0.0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0591966173361522</v>
+        <v>0.0551797040169133</v>
       </c>
       <c r="N5" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>6.68557644855895E-4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D6" t="n">
-        <v>29.0</v>
+        <v>141.0</v>
       </c>
       <c r="E6" t="n">
-        <v>26.0</v>
+        <v>34.0</v>
       </c>
       <c r="F6" t="n">
-        <v>4.2567941954014E-4</v>
+        <v>6.91424234824968E-40</v>
       </c>
       <c r="G6" t="n">
-        <v>7.27855148517323E-40</v>
+        <v>5.22572749966404E-38</v>
       </c>
       <c r="H6" t="n">
-        <v>1.34895703589137E-9</v>
+        <v>0.00511448636585391</v>
       </c>
       <c r="I6" t="n">
-        <v>65.0</v>
+        <v>66.0</v>
       </c>
       <c r="J6" t="n">
         <v>100.0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.07188160676532769</v>
       </c>
       <c r="L6" t="n">
         <v>0.0</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0551797040169133</v>
+        <v>0.0718816067653277</v>
       </c>
       <c r="N6" t="n">
-        <v>6.68557644855895E-4</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D7" t="n">
-        <v>48.0</v>
+        <v>103.0</v>
       </c>
       <c r="E7" t="n">
-        <v>15.0</v>
+        <v>19.0</v>
       </c>
       <c r="F7" t="n">
-        <v>6.35703372325376E-40</v>
+        <v>6.51999369723878E-40</v>
       </c>
       <c r="G7" t="n">
-        <v>5.55194292468331E-38</v>
+        <v>1.25468290861042E-39</v>
       </c>
       <c r="H7" t="n">
-        <v>0.00198021340048057</v>
+        <v>4.62499234591398E-4</v>
       </c>
       <c r="I7" t="n">
-        <v>64.0</v>
+        <v>65.0</v>
       </c>
       <c r="J7" t="n">
         <v>100.0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.03171247357293869</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="L7" t="n">
         <v>0.0</v>
       </c>
       <c r="M7" t="n">
-        <v>0.0317124735729387</v>
+        <v>0.040169133192389</v>
       </c>
       <c r="N7" t="n">
         <v>0.0</v>
@@ -3170,31 +3170,31 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D8" t="n">
-        <v>103.0</v>
+        <v>46.0</v>
       </c>
       <c r="E8" t="n">
         <v>19.0</v>
       </c>
       <c r="F8" t="n">
-        <v>6.51999369723878E-40</v>
+        <v>6.37169273862073E-40</v>
       </c>
       <c r="G8" t="n">
-        <v>1.25468290861042E-39</v>
+        <v>4.50672171343806E-36</v>
       </c>
       <c r="H8" t="n">
-        <v>4.62499234591398E-4</v>
+        <v>0.00625718664081437</v>
       </c>
       <c r="I8" t="n">
-        <v>62.0</v>
+        <v>63.0</v>
       </c>
       <c r="J8" t="n">
         <v>100.0</v>
@@ -3214,43 +3214,43 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
         <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="D9" t="n">
-        <v>141.0</v>
+        <v>48.0</v>
       </c>
       <c r="E9" t="n">
-        <v>34.0</v>
+        <v>15.0</v>
       </c>
       <c r="F9" t="n">
-        <v>6.91424234824968E-40</v>
+        <v>6.35703372325376E-40</v>
       </c>
       <c r="G9" t="n">
-        <v>5.22572749966404E-38</v>
+        <v>5.55194292468331E-38</v>
       </c>
       <c r="H9" t="n">
-        <v>0.00511448636585391</v>
+        <v>0.00198021340048057</v>
       </c>
       <c r="I9" t="n">
-        <v>55.0</v>
+        <v>62.0</v>
       </c>
       <c r="J9" t="n">
         <v>100.0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.07188160676532769</v>
+        <v>0.03171247357293869</v>
       </c>
       <c r="L9" t="n">
         <v>0.0</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0718816067653277</v>
+        <v>0.0317124735729387</v>
       </c>
       <c r="N9" t="n">
         <v>0.0</v>
@@ -3258,43 +3258,43 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>129</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
         <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="D10" t="n">
         <v>158.0</v>
       </c>
       <c r="E10" t="n">
-        <v>84.0</v>
+        <v>46.0</v>
       </c>
       <c r="F10" t="n">
-        <v>7.04377675145043E-40</v>
+        <v>6.81212204280953E-40</v>
       </c>
       <c r="G10" t="n">
-        <v>7.48419636793941E-40</v>
+        <v>1.08858185548109E-39</v>
       </c>
       <c r="H10" t="n">
-        <v>8.72881864945047E-5</v>
+        <v>5.24181844605938E-4</v>
       </c>
       <c r="I10" t="n">
-        <v>53.0</v>
+        <v>60.0</v>
       </c>
       <c r="J10" t="n">
         <v>100.0</v>
       </c>
       <c r="K10" t="n">
-        <v>0.179492600422833</v>
+        <v>0.09725158562367865</v>
       </c>
       <c r="L10" t="n">
-        <v>0.004280857659897791</v>
+        <v>0.0</v>
       </c>
       <c r="M10" t="n">
-        <v>0.177589852008457</v>
+        <v>0.0972515856236787</v>
       </c>
       <c r="N10" t="n">
         <v>0.0</v>
@@ -3302,40 +3302,40 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" t="n">
-        <v>93.0</v>
+        <v>158.0</v>
       </c>
       <c r="E11" t="n">
         <v>84.0</v>
       </c>
       <c r="F11" t="n">
-        <v>4.10865511869097E-15</v>
+        <v>7.04377675145043E-40</v>
       </c>
       <c r="G11" t="n">
-        <v>7.29044301902058E-40</v>
+        <v>7.48419636793941E-40</v>
       </c>
       <c r="H11" t="n">
-        <v>2.66335709542836E-4</v>
+        <v>8.72881864945047E-5</v>
       </c>
       <c r="I11" t="n">
-        <v>49.0</v>
+        <v>50.0</v>
       </c>
       <c r="J11" t="n">
         <v>100.0</v>
       </c>
       <c r="K11" t="n">
-        <v>0.179492600422833</v>
+        <v>0.17716701902748416</v>
       </c>
       <c r="L11" t="n">
-        <v>0.004280857659897791</v>
+        <v>0.0013371152897117948</v>
       </c>
       <c r="M11" t="n">
         <v>0.177589852008457</v>
@@ -3346,116 +3346,116 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="D12" t="n">
-        <v>250.0</v>
+        <v>32.0</v>
       </c>
       <c r="E12" t="n">
-        <v>26.0</v>
+        <v>2.0</v>
       </c>
       <c r="F12" t="n">
-        <v>6.81526409297973E-40</v>
+        <v>4.4059017720226E-40</v>
       </c>
       <c r="G12" t="n">
-        <v>1.07501177508528E-39</v>
+        <v>2.80388279688621E-39</v>
       </c>
       <c r="H12" t="n">
-        <v>0.00244603283957377</v>
+        <v>0.0</v>
       </c>
       <c r="I12" t="n">
-        <v>47.0</v>
+        <v>49.0</v>
       </c>
       <c r="J12" t="n">
         <v>100.0</v>
       </c>
       <c r="K12" t="n">
-        <v>0.05496828752642706</v>
+        <v>0.004228329809725159</v>
       </c>
       <c r="L12" t="n">
         <v>0.0</v>
       </c>
       <c r="M12" t="n">
-        <v>0.0549682875264271</v>
+        <v>0.00422832980972516</v>
       </c>
       <c r="N12" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>75</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="D13" t="n">
-        <v>46.0</v>
+        <v>34.0</v>
       </c>
       <c r="E13" t="n">
-        <v>19.0</v>
+        <v>29.0</v>
       </c>
       <c r="F13" t="n">
-        <v>6.37169273862073E-40</v>
+        <v>1.93777120033396E-6</v>
       </c>
       <c r="G13" t="n">
-        <v>4.50672171343806E-36</v>
+        <v>7.27702830087346E-40</v>
       </c>
       <c r="H13" t="n">
-        <v>0.00625718664081437</v>
+        <v>4.85557252274751E-5</v>
       </c>
       <c r="I13" t="n">
-        <v>46.0</v>
+        <v>47.0</v>
       </c>
       <c r="J13" t="n">
         <v>100.0</v>
       </c>
       <c r="K13" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0613107822410148</v>
       </c>
       <c r="L13" t="n">
         <v>0.0</v>
       </c>
       <c r="M13" t="n">
-        <v>0.040169133192389</v>
+        <v>0.0613107822410148</v>
       </c>
       <c r="N13" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>130</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="D14" t="n">
-        <v>158.0</v>
+        <v>93.0</v>
       </c>
       <c r="E14" t="n">
-        <v>46.0</v>
+        <v>84.0</v>
       </c>
       <c r="F14" t="n">
-        <v>6.81212204280953E-40</v>
+        <v>4.10865511869097E-15</v>
       </c>
       <c r="G14" t="n">
-        <v>1.08858185548109E-39</v>
+        <v>7.29044301902058E-40</v>
       </c>
       <c r="H14" t="n">
-        <v>5.24181844605938E-4</v>
+        <v>2.66335709542836E-4</v>
       </c>
       <c r="I14" t="n">
         <v>45.0</v>
@@ -3464,13 +3464,13 @@
         <v>100.0</v>
       </c>
       <c r="K14" t="n">
-        <v>0.09725158562367865</v>
+        <v>0.17716701902748416</v>
       </c>
       <c r="L14" t="n">
-        <v>0.0</v>
+        <v>0.0013371152897117948</v>
       </c>
       <c r="M14" t="n">
-        <v>0.0972515856236787</v>
+        <v>0.177589852008457</v>
       </c>
       <c r="N14" t="n">
         <v>0.0</v>
@@ -3478,87 +3478,87 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D15" t="n">
-        <v>34.0</v>
+        <v>26.0</v>
       </c>
       <c r="E15" t="n">
-        <v>29.0</v>
+        <v>25.0</v>
       </c>
       <c r="F15" t="n">
-        <v>1.93777120033396E-6</v>
+        <v>0.123041978875464</v>
       </c>
       <c r="G15" t="n">
-        <v>7.27702830087346E-40</v>
+        <v>7.64811423823189E-40</v>
       </c>
       <c r="H15" t="n">
-        <v>4.85557252274751E-5</v>
+        <v>1.57998188512074E-5</v>
       </c>
       <c r="I15" t="n">
-        <v>44.0</v>
+        <v>21.0</v>
       </c>
       <c r="J15" t="n">
         <v>100.0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.0613107822410148</v>
+        <v>0.052854122621564484</v>
       </c>
       <c r="L15" t="n">
         <v>0.0</v>
       </c>
       <c r="M15" t="n">
-        <v>0.0613107822410148</v>
+        <v>0.0528541226215645</v>
       </c>
       <c r="N15" t="n">
-        <v>3.2710259555912E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
         <v>77</v>
       </c>
-      <c r="C16" t="s">
-        <v>87</v>
-      </c>
       <c r="D16" t="n">
+        <v>250.0</v>
+      </c>
+      <c r="E16" t="n">
         <v>26.0</v>
       </c>
-      <c r="E16" t="n">
-        <v>25.0</v>
-      </c>
       <c r="F16" t="n">
-        <v>0.123041978875464</v>
+        <v>6.81526409297973E-40</v>
       </c>
       <c r="G16" t="n">
-        <v>7.64811423823189E-40</v>
+        <v>1.07501177508528E-39</v>
       </c>
       <c r="H16" t="n">
-        <v>1.57998188512074E-5</v>
+        <v>0.00244603283957377</v>
       </c>
       <c r="I16" t="n">
-        <v>41.0</v>
+        <v>20.0</v>
       </c>
       <c r="J16" t="n">
         <v>100.0</v>
       </c>
       <c r="K16" t="n">
-        <v>0.052854122621564484</v>
+        <v>0.05496828752642706</v>
       </c>
       <c r="L16" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M16" t="n">
-        <v>0.0528541226215645</v>
+        <v>0.0549682875264271</v>
       </c>
       <c r="N16" t="n">
         <v>0.0</v>
@@ -3566,43 +3566,43 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D17" t="n">
-        <v>120.0</v>
+        <v>265.0</v>
       </c>
       <c r="E17" t="n">
-        <v>82.0</v>
+        <v>23.0</v>
       </c>
       <c r="F17" t="n">
-        <v>8.41039238887027E-40</v>
+        <v>6.71457268463716E-40</v>
       </c>
       <c r="G17" t="n">
-        <v>7.87697455852087E-40</v>
+        <v>7.27946554528017E-40</v>
       </c>
       <c r="H17" t="n">
-        <v>7.20794801965287E-4</v>
+        <v>2.31452640435795E-4</v>
       </c>
       <c r="I17" t="n">
-        <v>30.0</v>
+        <v>18.0</v>
       </c>
       <c r="J17" t="n">
         <v>100.0</v>
       </c>
       <c r="K17" t="n">
-        <v>0.1733615221987315</v>
+        <v>0.048625792811839326</v>
       </c>
       <c r="L17" t="n">
         <v>0.0</v>
       </c>
       <c r="M17" t="n">
-        <v>0.173361522198731</v>
+        <v>0.0486257928118393</v>
       </c>
       <c r="N17" t="n">
         <v>0.0</v>
@@ -3610,43 +3610,43 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C18" t="s">
         <v>90</v>
       </c>
       <c r="D18" t="n">
-        <v>265.0</v>
+        <v>120.0</v>
       </c>
       <c r="E18" t="n">
-        <v>23.0</v>
+        <v>82.0</v>
       </c>
       <c r="F18" t="n">
-        <v>6.71457268463716E-40</v>
+        <v>8.41039238887027E-40</v>
       </c>
       <c r="G18" t="n">
-        <v>7.27946554528017E-40</v>
+        <v>7.87697455852087E-40</v>
       </c>
       <c r="H18" t="n">
-        <v>2.31452640435795E-4</v>
+        <v>7.20794801965287E-4</v>
       </c>
       <c r="I18" t="n">
-        <v>22.0</v>
+        <v>14.0</v>
       </c>
       <c r="J18" t="n">
         <v>100.0</v>
       </c>
       <c r="K18" t="n">
-        <v>0.048625792811839326</v>
+        <v>0.1733615221987315</v>
       </c>
       <c r="L18" t="n">
         <v>0.0</v>
       </c>
       <c r="M18" t="n">
-        <v>0.0486257928118393</v>
+        <v>0.173361522198731</v>
       </c>
       <c r="N18" t="n">
         <v>0.0</v>
@@ -3657,7 +3657,7 @@
         <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
         <v>91</v>
@@ -3678,7 +3678,7 @@
         <v>0.00115041602190713</v>
       </c>
       <c r="I19" t="n">
-        <v>18.0</v>
+        <v>9.0</v>
       </c>
       <c r="J19" t="n">
         <v>100.0</v>
@@ -3698,13 +3698,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D20" t="n">
         <v>48.0</v>
@@ -3742,7 +3742,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
         <v>66</v>
@@ -3781,12 +3781,12 @@
         <v>0.0570824524312896</v>
       </c>
       <c r="N21" t="n">
-        <v>0.0</v>
+        <v>2.31296463463574E-18</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
         <v>111</v>
@@ -3819,7 +3819,7 @@
         <v>0.05919661733615222</v>
       </c>
       <c r="L22" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M22" t="n">
         <v>0.0591966173361522</v>
@@ -3836,7 +3836,7 @@
         <v>66</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D23" t="n">
         <v>250.0</v>
@@ -3965,7 +3965,7 @@
         <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
         <v>93</v>
@@ -4001,12 +4001,12 @@
         <v>0.124735729386892</v>
       </c>
       <c r="N26" t="n">
-        <v>4.62592926927149E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B27" t="s">
         <v>73</v>
@@ -4045,12 +4045,12 @@
         <v>0.124735729386892</v>
       </c>
       <c r="N27" t="n">
-        <v>4.62592926927149E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>100</v>
@@ -4133,7 +4133,7 @@
         <v>0.0782241014799154</v>
       </c>
       <c r="N29" t="n">
-        <v>4.62592926927149E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="30">
@@ -4171,13 +4171,13 @@
         <v>0.05919661733615222</v>
       </c>
       <c r="L30" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M30" t="n">
         <v>0.0591966173361522</v>
       </c>
       <c r="N30" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31">
@@ -4185,7 +4185,7 @@
         <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C31" t="s">
         <v>95</v>
@@ -4215,7 +4215,7 @@
         <v>0.05919661733615222</v>
       </c>
       <c r="L31" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M31" t="n">
         <v>0.0591966173361522</v>
@@ -4259,13 +4259,13 @@
         <v>0.05919661733615222</v>
       </c>
       <c r="L32" t="n">
-        <v>0.0</v>
+        <v>2.3129646346357427E-18</v>
       </c>
       <c r="M32" t="n">
         <v>0.0591966173361522</v>
       </c>
       <c r="N32" t="n">
-        <v>3.2710259555912E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="33">
@@ -4276,7 +4276,7 @@
         <v>99</v>
       </c>
       <c r="C33" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D33" t="n">
         <v>31.0</v>
@@ -4303,13 +4303,13 @@
         <v>0.052854122621564484</v>
       </c>
       <c r="L33" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M33" t="n">
         <v>0.0528541226215645</v>
       </c>
       <c r="N33" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="34">
@@ -4320,7 +4320,7 @@
         <v>100</v>
       </c>
       <c r="C34" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D34" t="n">
         <v>64.0</v>
@@ -4347,7 +4347,7 @@
         <v>0.052854122621564484</v>
       </c>
       <c r="L34" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M34" t="n">
         <v>0.0528541226215645</v>
@@ -4358,13 +4358,13 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
         <v>78</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D35" t="n">
         <v>120.0</v>
@@ -4391,13 +4391,13 @@
         <v>0.052854122621564484</v>
       </c>
       <c r="L35" t="n">
-        <v>2.3129646346357427E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M35" t="n">
         <v>0.0528541226215645</v>
       </c>
       <c r="N35" t="n">
-        <v>3.2710259555912E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="36">
@@ -4408,7 +4408,7 @@
         <v>100</v>
       </c>
       <c r="C36" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D36" t="n">
         <v>64.0</v>
@@ -4435,7 +4435,7 @@
         <v>0.06765327695560254</v>
       </c>
       <c r="L36" t="n">
-        <v>6.542051911182396E-18</v>
+        <v>0.0</v>
       </c>
       <c r="M36" t="n">
         <v>0.0676532769556025</v>
@@ -4449,10 +4449,10 @@
         <v>14</v>
       </c>
       <c r="B37" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D37" t="n">
         <v>84.0</v>
@@ -4490,13 +4490,13 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B38" t="s">
         <v>95</v>
       </c>
       <c r="C38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D38" t="n">
         <v>28.0</v>
@@ -4540,7 +4540,7 @@
         <v>96</v>
       </c>
       <c r="C39" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D39" t="n">
         <v>41.0</v>
@@ -4584,7 +4584,7 @@
         <v>99</v>
       </c>
       <c r="C40" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D40" t="n">
         <v>31.0</v>
@@ -4625,7 +4625,7 @@
         <v>50</v>
       </c>
       <c r="B41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C41" t="s">
         <v>98</v>
@@ -4669,7 +4669,7 @@
         <v>51</v>
       </c>
       <c r="B42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C42" t="s">
         <v>98</v>
@@ -4713,7 +4713,7 @@
         <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C43" t="s">
         <v>99</v>
@@ -4743,13 +4743,13 @@
         <v>0.06553911205073996</v>
       </c>
       <c r="L43" t="n">
-        <v>4.625929269271485E-18</v>
+        <v>8.012344526598183E-18</v>
       </c>
       <c r="M43" t="n">
         <v>0.06553911205074</v>
       </c>
       <c r="N43" t="n">
-        <v>4.62592926927149E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="44">
@@ -4757,7 +4757,7 @@
         <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C44" t="s">
         <v>100</v>
@@ -4875,13 +4875,13 @@
         <v>0.05708245243128964</v>
       </c>
       <c r="L46" t="n">
-        <v>0.0</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M46" t="n">
         <v>0.0570824524312896</v>
       </c>
       <c r="N46" t="n">
-        <v>2.31296463463574E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="47">
@@ -4919,7 +4919,7 @@
         <v>0.05708245243128964</v>
       </c>
       <c r="L47" t="n">
-        <v>0.0</v>
+        <v>3.271025955591198E-18</v>
       </c>
       <c r="M47" t="n">
         <v>0.0570824524312896</v>
@@ -4977,10 +4977,10 @@
         <v>60</v>
       </c>
       <c r="B49" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D49" t="n">
         <v>46.0</v>
@@ -5021,10 +5021,10 @@
         <v>61</v>
       </c>
       <c r="B50" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D50" t="n">
         <v>93.0</v>
@@ -5065,7 +5065,7 @@
         <v>63</v>
       </c>
       <c r="B51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C51" t="s">
         <v>77</v>
@@ -5101,7 +5101,7 @@
         <v>0.0549682875264271</v>
       </c>
       <c r="N51" t="n">
-        <v>3.2710259555912E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="52">
@@ -5197,10 +5197,10 @@
         <v>133</v>
       </c>
       <c r="B54" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C54" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D54" t="n">
         <v>93.0</v>
@@ -5244,7 +5244,7 @@
         <v>66</v>
       </c>
       <c r="C55" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D55" t="n">
         <v>250.0</v>
@@ -5277,7 +5277,7 @@
         <v>0.101479915433404</v>
       </c>
       <c r="N55" t="n">
-        <v>4.62592926927149E-18</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="56">
@@ -5288,7 +5288,7 @@
         <v>66</v>
       </c>
       <c r="C56" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D56" t="n">
         <v>250.0</v>
@@ -5417,7 +5417,7 @@
         <v>138</v>
       </c>
       <c r="B59" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C59" t="s">
         <v>114</v>
@@ -5461,7 +5461,7 @@
         <v>139</v>
       </c>
       <c r="B60" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C60" t="s">
         <v>114</v>
@@ -5502,7 +5502,7 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B61" t="s">
         <v>79</v>
@@ -5546,7 +5546,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B62" t="s">
         <v>79</v>
@@ -5590,7 +5590,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B63" t="s">
         <v>79</v>
@@ -5640,7 +5640,7 @@
         <v>79</v>
       </c>
       <c r="C64" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D64" t="e">
         <v>#NUM!</v>
@@ -5678,13 +5678,13 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B65" t="s">
         <v>79</v>
       </c>
       <c r="C65" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D65" t="e">
         <v>#NUM!</v>
@@ -5860,7 +5860,7 @@
         <v>79</v>
       </c>
       <c r="C69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D69" t="e">
         <v>#NUM!</v>
@@ -5928,10 +5928,10 @@
         <v>#NUM!</v>
       </c>
       <c r="K70" t="n">
-        <v>0.48414376321353064</v>
+        <v>0.49217758985200843</v>
       </c>
       <c r="L70" t="n">
-        <v>0.0</v>
+        <v>0.01693679366968268</v>
       </c>
       <c r="M70" t="e">
         <v>#NUM!</v>

</xml_diff>